<commit_message>
Bones -> Dislocation -> All, Bones -> Fracture -> All
</commit_message>
<xml_diff>
--- a/Chest Findings Reicher Wu 1_18_2018 (Autosaved).xlsx
+++ b/Chest Findings Reicher Wu 1_18_2018 (Autosaved).xlsx
@@ -4000,8 +4000,8 @@
   <dimension ref="A1:O344"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C348" sqref="C348"/>
+      <pane ySplit="1" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A240" sqref="A240:XFD240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12877,7 +12877,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="238" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>4</v>
       </c>
@@ -12918,7 +12918,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="239" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>4</v>
       </c>
@@ -12959,7 +12959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="240" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>4</v>
       </c>
@@ -13000,7 +13000,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="241" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>4</v>
       </c>
@@ -13041,7 +13041,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="242" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>4</v>
       </c>
@@ -13082,7 +13082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="243" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>4</v>
       </c>
@@ -13121,7 +13121,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="244" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>4</v>
       </c>
@@ -13160,7 +13160,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="245" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>4</v>
       </c>
@@ -13199,7 +13199,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="246" spans="1:15" ht="44.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:15" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>4</v>
       </c>
@@ -13238,7 +13238,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="247" spans="1:15" ht="42.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:15" ht="42.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>4</v>
       </c>
@@ -13277,7 +13277,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="248" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>4</v>
       </c>
@@ -13316,7 +13316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="249" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>4</v>
       </c>
@@ -13355,7 +13355,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="250" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>4</v>
       </c>
@@ -13396,7 +13396,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="251" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
         <v>4</v>
       </c>
@@ -13437,7 +13437,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="252" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>4</v>
       </c>
@@ -13478,7 +13478,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="253" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>4</v>
       </c>
@@ -13519,7 +13519,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="254" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>4</v>
       </c>
@@ -13560,7 +13560,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="255" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>4</v>
       </c>
@@ -13599,7 +13599,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="256" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>4</v>
       </c>
@@ -13638,7 +13638,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="257" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
         <v>4</v>
       </c>
@@ -13677,7 +13677,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="258" spans="1:15" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:15" ht="44.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
         <v>4</v>
       </c>
@@ -13716,7 +13716,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="259" spans="1:15" ht="42.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:15" ht="42.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>4</v>
       </c>
@@ -13755,7 +13755,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="260" spans="1:15" ht="60" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
         <v>4</v>
       </c>
@@ -13794,7 +13794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="261" spans="1:15" ht="60" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>4</v>
       </c>
@@ -16870,7 +16870,7 @@
     </filterColumn>
     <filterColumn colId="1">
       <filters>
-        <filter val="Bone lesion"/>
+        <filter val="Fracture"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Bones -> Metal Bone -> All
Bones -> Scoliosis -> All and Bones -> Spinal Degen -> All
</commit_message>
<xml_diff>
--- a/Chest Findings Reicher Wu 1_18_2018 (Autosaved).xlsx
+++ b/Chest Findings Reicher Wu 1_18_2018 (Autosaved).xlsx
@@ -3999,9 +3999,9 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:O344"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A240" sqref="A240:XFD240"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A274" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J357" sqref="J357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12877,7 +12877,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="238" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>4</v>
       </c>
@@ -12918,7 +12918,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="239" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>4</v>
       </c>
@@ -12959,7 +12959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="240" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>4</v>
       </c>
@@ -13000,7 +13000,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="241" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>4</v>
       </c>
@@ -13041,7 +13041,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="242" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>4</v>
       </c>
@@ -13082,7 +13082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="243" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>4</v>
       </c>
@@ -13121,7 +13121,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="244" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>4</v>
       </c>
@@ -13160,7 +13160,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="245" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>4</v>
       </c>
@@ -13199,7 +13199,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="246" spans="1:15" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:15" ht="44.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>4</v>
       </c>
@@ -13238,7 +13238,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="247" spans="1:15" ht="42.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:15" ht="42.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>4</v>
       </c>
@@ -13277,7 +13277,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="248" spans="1:15" ht="60" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>4</v>
       </c>
@@ -13316,7 +13316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="249" spans="1:15" ht="60" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>4</v>
       </c>
@@ -14275,7 +14275,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="274" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>4</v>
       </c>
@@ -14315,7 +14315,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="275" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
         <v>4</v>
       </c>
@@ -14355,7 +14355,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="276" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>4</v>
       </c>
@@ -16870,7 +16870,7 @@
     </filterColumn>
     <filterColumn colId="1">
       <filters>
-        <filter val="Fracture"/>
+        <filter val="Scoliosis"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Lungs -> Alveolar, Lungs -> Atelectasis
</commit_message>
<xml_diff>
--- a/Chest Findings Reicher Wu 1_18_2018 (Autosaved).xlsx
+++ b/Chest Findings Reicher Wu 1_18_2018 (Autosaved).xlsx
@@ -3999,9 +3999,9 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:O344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A274" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J357" sqref="J357"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H347" sqref="H347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5124,7 +5124,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -14275,7 +14275,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="274" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>4</v>
       </c>
@@ -14315,7 +14315,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="275" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
         <v>4</v>
       </c>
@@ -14355,7 +14355,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="276" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>4</v>
       </c>
@@ -16865,12 +16865,17 @@
   <autoFilter ref="A1:O343">
     <filterColumn colId="0">
       <filters>
-        <filter val="Bones"/>
+        <filter val="Lungs"/>
       </filters>
     </filterColumn>
     <filterColumn colId="1">
       <filters>
-        <filter val="Scoliosis"/>
+        <filter val="Alveolar opacity"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="All lung zones"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Lungs -> Enlarged Hilum, Granulomatous, Granulomatous disease
</commit_message>
<xml_diff>
--- a/Chest Findings Reicher Wu 1_18_2018 (Autosaved).xlsx
+++ b/Chest Findings Reicher Wu 1_18_2018 (Autosaved).xlsx
@@ -4000,8 +4000,8 @@
   <dimension ref="A1:O344"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H347" sqref="H347"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5124,7 +5124,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -6546,7 +6546,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
@@ -6654,7 +6654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -16870,12 +16870,7 @@
     </filterColumn>
     <filterColumn colId="1">
       <filters>
-        <filter val="Alveolar opacity"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="All lung zones"/>
+        <filter val="findings consistent with granulomatous disease"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Major Airways - > All
</commit_message>
<xml_diff>
--- a/Chest Findings Reicher Wu 1_18_2018 (Autosaved).xlsx
+++ b/Chest Findings Reicher Wu 1_18_2018 (Autosaved).xlsx
@@ -4000,8 +4000,8 @@
   <dimension ref="A1:O344"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
+      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B152" sqref="A152:XFD153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5664,7 +5664,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="70.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="70.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="70.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="70.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -5790,7 +5790,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -5958,7 +5958,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -6000,7 +6000,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>2</v>
       </c>
@@ -9722,7 +9722,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>2</v>
       </c>
@@ -9759,7 +9759,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="156" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>2</v>
       </c>
@@ -9798,7 +9798,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>2</v>
       </c>
@@ -9837,7 +9837,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>2</v>
       </c>
@@ -9874,7 +9874,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>2</v>
       </c>
@@ -9911,7 +9911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>2</v>
       </c>
@@ -9948,7 +9948,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>2</v>
       </c>
@@ -9985,7 +9985,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>2</v>
       </c>
@@ -10021,7 +10021,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="163" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>2</v>
       </c>
@@ -10058,7 +10058,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>2</v>
       </c>
@@ -10095,7 +10095,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="165" spans="1:15" ht="45.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:15" ht="45.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>2</v>
       </c>
@@ -10132,7 +10132,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>2</v>
       </c>
@@ -10168,7 +10168,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>2</v>
       </c>
@@ -10204,7 +10204,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="168" spans="1:15" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>2</v>
       </c>
@@ -10240,7 +10240,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="169" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>2</v>
       </c>
@@ -10276,7 +10276,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="170" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>2</v>
       </c>
@@ -10312,7 +10312,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="171" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>2</v>
       </c>
@@ -10348,7 +10348,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>2</v>
       </c>
@@ -10384,7 +10384,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="173" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>2</v>
       </c>
@@ -10420,7 +10420,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="174" spans="1:15" ht="44.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:15" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>2</v>
       </c>
@@ -10456,7 +10456,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>2</v>
       </c>
@@ -10492,7 +10492,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="176" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>2</v>
       </c>
@@ -10528,7 +10528,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="177" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>2</v>
       </c>
@@ -10564,7 +10564,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>2</v>
       </c>
@@ -10600,7 +10600,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="179" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>2</v>
       </c>
@@ -10636,7 +10636,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>2</v>
       </c>
@@ -10672,7 +10672,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="181" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>2</v>
       </c>
@@ -10708,7 +10708,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="182" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>2</v>
       </c>
@@ -10744,7 +10744,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="183" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>2</v>
       </c>
@@ -10780,7 +10780,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>2</v>
       </c>
@@ -10816,7 +10816,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>2</v>
       </c>
@@ -10852,7 +10852,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>2</v>
       </c>
@@ -16865,12 +16865,7 @@
   <autoFilter ref="A1:O343">
     <filterColumn colId="0">
       <filters>
-        <filter val="Lungs"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Mass/Nodule"/>
+        <filter val="Mediastinum"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>